<commit_message>
solved need is graph
</commit_message>
<xml_diff>
--- a/where_is_inventry.xlsx
+++ b/where_is_inventry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyle\Desktop\git_repository\imagine_warehouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EF0ABA-1CA6-4390-81B1-40E0553413DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B958483-ACF2-4B05-8164-674A12EE42A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>